<commit_message>
push files to github
</commit_message>
<xml_diff>
--- a/sql/Field Config.xlsx
+++ b/sql/Field Config.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\Desktop\Fortune Queries\Assignment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\data-engg\data_engineer_assessment\sql\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6A78F5D2-DF28-43DF-ABB6-6EAA3DECAD84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="19380" windowHeight="20970" xr2:uid="{21BE63E6-2E88-4952-BBE6-C1795A0D8A81}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="19380" windowHeight="20976"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -249,7 +248,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -609,20 +608,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24DCFBAE-81BF-4BF4-BADA-C81DFB5B08C4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="248" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="A8" sqref="A1:B67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.54296875" customWidth="1"/>
+    <col min="1" max="1" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>72</v>
       </c>
@@ -630,7 +629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -638,7 +637,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -646,7 +645,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -654,7 +653,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -662,7 +661,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -670,7 +669,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -678,7 +677,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -686,7 +685,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -694,7 +693,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -702,7 +701,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -710,7 +709,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -718,7 +717,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -726,7 +725,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -734,7 +733,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -742,7 +741,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -750,7 +749,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -758,7 +757,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -766,7 +765,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -774,7 +773,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>27</v>
       </c>
@@ -782,7 +781,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>28</v>
       </c>
@@ -790,7 +789,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>29</v>
       </c>
@@ -798,7 +797,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>30</v>
       </c>
@@ -806,7 +805,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -814,7 +813,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>31</v>
       </c>
@@ -822,7 +821,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>9</v>
       </c>
@@ -830,7 +829,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>10</v>
       </c>
@@ -838,7 +837,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>32</v>
       </c>
@@ -846,7 +845,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>33</v>
       </c>
@@ -854,7 +853,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>34</v>
       </c>
@@ -862,7 +861,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>35</v>
       </c>
@@ -870,7 +869,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>36</v>
       </c>
@@ -878,7 +877,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>37</v>
       </c>
@@ -886,7 +885,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>38</v>
       </c>
@@ -894,7 +893,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>15</v>
       </c>
@@ -902,7 +901,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>39</v>
       </c>
@@ -910,7 +909,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>40</v>
       </c>
@@ -918,7 +917,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>41</v>
       </c>
@@ -926,7 +925,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>42</v>
       </c>
@@ -934,7 +933,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>43</v>
       </c>
@@ -942,7 +941,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>44</v>
       </c>
@@ -950,7 +949,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>45</v>
       </c>
@@ -958,7 +957,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>46</v>
       </c>
@@ -966,7 +965,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>47</v>
       </c>
@@ -974,7 +973,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>48</v>
       </c>
@@ -982,7 +981,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>49</v>
       </c>
@@ -990,7 +989,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>50</v>
       </c>
@@ -998,7 +997,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>51</v>
       </c>
@@ -1006,7 +1005,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>52</v>
       </c>
@@ -1014,7 +1013,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>53</v>
       </c>
@@ -1022,7 +1021,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>54</v>
       </c>
@@ -1030,7 +1029,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>55</v>
       </c>
@@ -1038,7 +1037,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>56</v>
       </c>
@@ -1046,7 +1045,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>57</v>
       </c>
@@ -1054,7 +1053,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>58</v>
       </c>
@@ -1062,7 +1061,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>59</v>
       </c>
@@ -1070,7 +1069,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>60</v>
       </c>
@@ -1078,7 +1077,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>12</v>
       </c>
@@ -1086,7 +1085,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>13</v>
       </c>
@@ -1094,7 +1093,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>11</v>
       </c>
@@ -1102,7 +1101,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>61</v>
       </c>
@@ -1110,7 +1109,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>62</v>
       </c>
@@ -1118,7 +1117,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>63</v>
       </c>
@@ -1126,7 +1125,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>64</v>
       </c>
@@ -1134,7 +1133,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>65</v>
       </c>
@@ -1142,7 +1141,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>66</v>
       </c>
@@ -1150,7 +1149,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>67</v>
       </c>

</xml_diff>